<commit_message>
Introducing copy action and constants module
</commit_message>
<xml_diff>
--- a/tests/_resources/example.xlsx
+++ b/tests/_resources/example.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Move</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>/source-directory/c/e/data</t>
+  </si>
+  <si>
+    <t>Copy</t>
   </si>
 </sst>
 </file>
@@ -440,18 +443,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="26" width="8.6640625" style="1" customWidth="1"/>
     <col min="27" max="16384" width="14.44140625" style="1"/>
   </cols>
@@ -565,7 +568,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>21</v>
@@ -1542,7 +1545,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E14">
-      <formula1>"Not defined,Move,Delete"</formula1>
+      <formula1>"Not defined,Copy,Move,Delete"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>